<commit_message>
TRANSLATE-2072 move character pixel definition from customer to file level - ("migration":) use pixelMapping from Spreadsheet for task instead of linking it to customers
</commit_message>
<xml_diff>
--- a/application/modules/editor/testcases/editorAPI/XlfSegmentLinesPixelLengthTest/testfiles/pixel-mapping.xlsx
+++ b/application/modules/editor/testcases/editorAPI/XlfSegmentLinesPixelLengthTest/testfiles/pixel-mapping.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
-  <si>
-    <t xml:space="preserve">clientNumber</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t xml:space="preserve">font</t>
   </si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">default for legacy data</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
@@ -159,12 +153,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -174,19 +168,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:AMJ10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A5"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.03"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.03"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="4" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -202,202 +196,173 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>6</v>
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>123456789</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>13</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>14</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>72</v>
-      </c>
-      <c r="E9" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
+      <c r="E9" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>83</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" display="See https://en.wikipedia.org/wiki/List_of_Unicode_characters"/>
+    <hyperlink ref="G3" r:id="rId1" display="See https://en.wikipedia.org/wiki/List_of_Unicode_characters"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>